<commit_message>
Update the conversion check xlsx
</commit_message>
<xml_diff>
--- a/src/conversion check.xlsx
+++ b/src/conversion check.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\install location\java\work\joseph final\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\main\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8160"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21576" windowHeight="8160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>floated</t>
   </si>
@@ -78,13 +78,16 @@
   </si>
   <si>
     <t>edit 1-d-1 april -1a-c-c</t>
+  </si>
+  <si>
+    <t>set file location -new_path</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -395,15 +398,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C4:K14"/>
+  <dimension ref="C4:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="4" spans="3:11">
+    <row r="4" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
         <v>0</v>
       </c>
@@ -414,7 +417,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="3:11">
+    <row r="5" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
         <v>3</v>
       </c>
@@ -425,7 +428,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="3:11">
+    <row r="9" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
         <v>6</v>
       </c>
@@ -436,7 +439,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="3:11">
+    <row r="10" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
         <v>8</v>
       </c>
@@ -447,7 +450,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="3:11">
+    <row r="13" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
         <v>7</v>
       </c>
@@ -458,7 +461,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="3:11">
+    <row r="14" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
         <v>16</v>
       </c>
@@ -467,6 +470,11 @@
       </c>
       <c r="K14" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C18" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>